<commit_message>
Actualizarion pisos.com, clustering chatgpt
</commit_message>
<xml_diff>
--- a/codigo/01-preprocesamiento-de-datos/02-datos-limpios/distr_barrios_codpostal.xlsx
+++ b/codigo/01-preprocesamiento-de-datos/02-datos-limpios/distr_barrios_codpostal.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\extas\Documents\GitHub\precios-de-vivienda-madrid\codigo\01-preprocesamiento-de-datos\02-datos-limpios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2908E08-0F1B-466F-A90C-F7AC9F098DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED8180A4-E7E3-4D22-9FFB-87FBB8282748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="159">
   <si>
     <t>cod_distrito</t>
   </si>
@@ -385,9 +385,6 @@
     <t>Atalaya</t>
   </si>
   <si>
-    <t>Costezuela</t>
-  </si>
-  <si>
     <t>Hortaleza</t>
   </si>
   <si>
@@ -503,17 +500,37 @@
   </si>
   <si>
     <t>Villaverde Alto</t>
+  </si>
+  <si>
+    <t>Casco Histórico de Barajas</t>
+  </si>
+  <si>
+    <t>Costillares</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -570,12 +587,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -796,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:XFD34"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -816,7 +835,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -825,7 +844,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
@@ -2824,8 +2843,8 @@
       <c r="D101" s="2">
         <v>9</v>
       </c>
-      <c r="E101" s="2" t="s">
-        <v>118</v>
+      <c r="E101" s="7" t="s">
+        <v>158</v>
       </c>
       <c r="F101" s="2">
         <v>28027</v>
@@ -2836,7 +2855,7 @@
         <v>16</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C102" s="2">
         <v>161</v>
@@ -2845,7 +2864,7 @@
         <v>1</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F102" s="2">
         <v>28043</v>
@@ -2856,7 +2875,7 @@
         <v>16</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C103" s="2">
         <v>162</v>
@@ -2865,7 +2884,7 @@
         <v>2</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F103" s="2">
         <v>28055</v>
@@ -2876,7 +2895,7 @@
         <v>16</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C104" s="2">
         <v>163</v>
@@ -2885,7 +2904,7 @@
         <v>3</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F104" s="2">
         <v>28043</v>
@@ -2896,7 +2915,7 @@
         <v>16</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C105" s="2">
         <v>164</v>
@@ -2905,7 +2924,7 @@
         <v>4</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F105" s="2">
         <v>28033</v>
@@ -2916,7 +2935,7 @@
         <v>16</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C106" s="2">
         <v>165</v>
@@ -2925,7 +2944,7 @@
         <v>5</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F106" s="2">
         <v>28033</v>
@@ -2936,7 +2955,7 @@
         <v>16</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C107" s="2">
         <v>166</v>
@@ -2945,7 +2964,7 @@
         <v>6</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F107" s="2">
         <v>28033</v>
@@ -2956,7 +2975,7 @@
         <v>16</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C108" s="2">
         <v>167</v>
@@ -2965,7 +2984,7 @@
         <v>7</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F108" s="2">
         <v>28055</v>
@@ -2976,7 +2995,7 @@
         <v>17</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C109" s="2">
         <v>171</v>
@@ -2985,7 +3004,7 @@
         <v>1</v>
       </c>
       <c r="E109" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F109" s="2">
         <v>28021</v>
@@ -2996,7 +3015,7 @@
         <v>17</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C110" s="2">
         <v>172</v>
@@ -3005,7 +3024,7 @@
         <v>2</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F110" s="2">
         <v>28021</v>
@@ -3016,7 +3035,7 @@
         <v>17</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C111" s="2">
         <v>173</v>
@@ -3025,7 +3044,7 @@
         <v>3</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F111" s="2">
         <v>28021</v>
@@ -3036,7 +3055,7 @@
         <v>17</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C112" s="2">
         <v>174</v>
@@ -3045,7 +3064,7 @@
         <v>4</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F112" s="2">
         <v>28021</v>
@@ -3056,7 +3075,7 @@
         <v>17</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C113" s="2">
         <v>175</v>
@@ -3065,7 +3084,7 @@
         <v>5</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F113" s="2">
         <v>28021</v>
@@ -3076,7 +3095,7 @@
         <v>18</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C114" s="2">
         <v>181</v>
@@ -3085,7 +3104,7 @@
         <v>1</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F114" s="2">
         <v>28031</v>
@@ -3096,7 +3115,7 @@
         <v>18</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C115" s="2">
         <v>182</v>
@@ -3105,7 +3124,7 @@
         <v>2</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F115" s="2">
         <v>28031</v>
@@ -3116,7 +3135,7 @@
         <v>18</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C116" s="2">
         <v>183</v>
@@ -3125,7 +3144,7 @@
         <v>3</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F116" s="2">
         <v>28031</v>
@@ -3136,7 +3155,7 @@
         <v>19</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C117" s="2">
         <v>191</v>
@@ -3145,7 +3164,7 @@
         <v>1</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F117" s="2">
         <v>28032</v>
@@ -3156,7 +3175,7 @@
         <v>19</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C118" s="2">
         <v>192</v>
@@ -3165,7 +3184,7 @@
         <v>2</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F118" s="2">
         <v>28032</v>
@@ -3176,7 +3195,7 @@
         <v>19</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C119" s="2">
         <v>193</v>
@@ -3185,7 +3204,7 @@
         <v>3</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F119" s="2">
         <v>28032</v>
@@ -3196,7 +3215,7 @@
         <v>19</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C120" s="2">
         <v>194</v>
@@ -3205,7 +3224,7 @@
         <v>4</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F120" s="2">
         <v>28032</v>
@@ -3216,7 +3235,7 @@
         <v>20</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C121" s="2">
         <v>201</v>
@@ -3225,7 +3244,7 @@
         <v>1</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F121" s="2">
         <v>28037</v>
@@ -3236,7 +3255,7 @@
         <v>20</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C122" s="2">
         <v>202</v>
@@ -3245,7 +3264,7 @@
         <v>2</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F122" s="2">
         <v>28037</v>
@@ -3256,7 +3275,7 @@
         <v>20</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C123" s="2">
         <v>203</v>
@@ -3265,7 +3284,7 @@
         <v>3</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F123" s="2">
         <v>28037</v>
@@ -3276,7 +3295,7 @@
         <v>20</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C124" s="2">
         <v>204</v>
@@ -3285,7 +3304,7 @@
         <v>4</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F124" s="2">
         <v>28037</v>
@@ -3296,7 +3315,7 @@
         <v>20</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C125" s="2">
         <v>205</v>
@@ -3305,7 +3324,7 @@
         <v>5</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F125" s="2">
         <v>28037</v>
@@ -3316,7 +3335,7 @@
         <v>20</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C126" s="2">
         <v>206</v>
@@ -3325,7 +3344,7 @@
         <v>6</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F126" s="2">
         <v>28037</v>
@@ -3337,7 +3356,7 @@
         <v>20</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C127" s="2">
         <v>207</v>
@@ -3346,7 +3365,7 @@
         <v>7</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F127" s="2">
         <v>28037</v>
@@ -3358,7 +3377,7 @@
         <v>20</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C128" s="2">
         <v>208</v>
@@ -3367,7 +3386,7 @@
         <v>8</v>
       </c>
       <c r="E128" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F128" s="2">
         <v>28037</v>
@@ -3378,7 +3397,7 @@
         <v>21</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C129" s="2">
         <v>211</v>
@@ -3387,7 +3406,7 @@
         <v>1</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F129" s="2">
         <v>28042</v>
@@ -3398,7 +3417,7 @@
         <v>21</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C130" s="2">
         <v>212</v>
@@ -3407,7 +3426,7 @@
         <v>2</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F130" s="2">
         <v>28042</v>
@@ -3418,7 +3437,7 @@
         <v>21</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C131" s="2">
         <v>213</v>
@@ -3426,8 +3445,8 @@
       <c r="D131" s="2">
         <v>3</v>
       </c>
-      <c r="E131" s="2" t="s">
-        <v>152</v>
+      <c r="E131" s="6" t="s">
+        <v>157</v>
       </c>
       <c r="F131" s="2">
         <v>28042</v>
@@ -3438,7 +3457,7 @@
         <v>21</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C132" s="2">
         <v>214</v>
@@ -3447,13 +3466,32 @@
         <v>4</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F132" s="2">
         <v>28042</v>
       </c>
     </row>
-    <row r="133" spans="1:6" ht="14.25" customHeight="1"/>
+    <row r="133" spans="1:6" ht="14.25" customHeight="1">
+      <c r="A133" s="1">
+        <v>21</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C133" s="2">
+        <v>215</v>
+      </c>
+      <c r="D133" s="2">
+        <v>5</v>
+      </c>
+      <c r="E133" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="F133" s="2">
+        <v>28042</v>
+      </c>
+    </row>
     <row r="134" spans="1:6" ht="14.25" customHeight="1"/>
     <row r="135" spans="1:6" ht="14.25" customHeight="1"/>
     <row r="136" spans="1:6" ht="14.25" customHeight="1"/>

</xml_diff>